<commit_message>
Aggiunge script aggiornato nella costruzione control set con k=1
</commit_message>
<xml_diff>
--- a/output/B_vector_diag.xlsx
+++ b/output/B_vector_diag.xlsx
@@ -467,7 +467,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -517,7 +517,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -562,7 +562,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -572,7 +572,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -657,7 +657,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -702,7 +702,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -737,12 +737,12 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -767,7 +767,7 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -967,7 +967,7 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -977,7 +977,7 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -1022,7 +1022,7 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -1037,7 +1037,7 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -1087,7 +1087,7 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -1112,7 +1112,7 @@
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -1212,7 +1212,7 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -1232,7 +1232,7 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -1282,7 +1282,7 @@
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -1292,27 +1292,27 @@
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177">
@@ -1392,7 +1392,7 @@
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -1407,7 +1407,7 @@
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -1422,7 +1422,7 @@
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -1522,7 +1522,7 @@
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219">
@@ -1737,22 +1737,22 @@
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265">
@@ -1772,7 +1772,7 @@
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="269">
@@ -1907,17 +1907,17 @@
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="298">
@@ -1942,7 +1942,7 @@
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="303">
@@ -2037,12 +2037,12 @@
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="323">
@@ -2057,7 +2057,7 @@
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="326">
@@ -2082,7 +2082,7 @@
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="331">
@@ -2092,7 +2092,7 @@
     </row>
     <row r="332">
       <c r="A332" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="333">
@@ -2147,12 +2147,12 @@
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="345">
@@ -2352,7 +2352,7 @@
     </row>
     <row r="384">
       <c r="A384" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="385">
@@ -2377,17 +2377,17 @@
     </row>
     <row r="389">
       <c r="A389" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="392">
@@ -2402,7 +2402,7 @@
     </row>
     <row r="394">
       <c r="A394" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="395">
@@ -2432,7 +2432,7 @@
     </row>
     <row r="400">
       <c r="A400" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="401">
@@ -2452,7 +2452,7 @@
     </row>
     <row r="404">
       <c r="A404" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="405">
@@ -2472,7 +2472,7 @@
     </row>
     <row r="408">
       <c r="A408" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="409">
@@ -2512,7 +2512,7 @@
     </row>
     <row r="416">
       <c r="A416" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="417">
@@ -2597,7 +2597,7 @@
     </row>
     <row r="433">
       <c r="A433" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="434">
@@ -2657,7 +2657,7 @@
     </row>
     <row r="445">
       <c r="A445" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="446">
@@ -2692,7 +2692,7 @@
     </row>
     <row r="452">
       <c r="A452" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="453">
@@ -2702,7 +2702,7 @@
     </row>
     <row r="454">
       <c r="A454" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="455">
@@ -2727,7 +2727,7 @@
     </row>
     <row r="459">
       <c r="A459" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="460">
@@ -2792,7 +2792,7 @@
     </row>
     <row r="472">
       <c r="A472" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="473">
@@ -2802,12 +2802,12 @@
     </row>
     <row r="474">
       <c r="A474" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="475">
       <c r="A475" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="476">
@@ -2907,7 +2907,7 @@
     </row>
     <row r="495">
       <c r="A495" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="496">
@@ -3172,7 +3172,7 @@
     </row>
     <row r="548">
       <c r="A548" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="549">
@@ -3412,7 +3412,7 @@
     </row>
     <row r="596">
       <c r="A596" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="597">
@@ -3482,7 +3482,7 @@
     </row>
     <row r="610">
       <c r="A610" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="611">
@@ -3547,7 +3547,7 @@
     </row>
     <row r="623">
       <c r="A623" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="624">
@@ -3562,7 +3562,7 @@
     </row>
     <row r="626">
       <c r="A626" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="627">
@@ -3702,7 +3702,7 @@
     </row>
     <row r="654">
       <c r="A654" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="655">
@@ -3727,7 +3727,7 @@
     </row>
     <row r="659">
       <c r="A659" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="660">
@@ -3767,7 +3767,7 @@
     </row>
     <row r="667">
       <c r="A667" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="668">
@@ -3862,7 +3862,7 @@
     </row>
     <row r="686">
       <c r="A686" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="687">
@@ -3882,7 +3882,7 @@
     </row>
     <row r="690">
       <c r="A690" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="691">
@@ -4052,7 +4052,7 @@
     </row>
     <row r="724">
       <c r="A724" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="725">
@@ -4152,7 +4152,7 @@
     </row>
     <row r="744">
       <c r="A744" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="745">
@@ -4247,7 +4247,7 @@
     </row>
     <row r="763">
       <c r="A763" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="764">
@@ -4367,7 +4367,7 @@
     </row>
     <row r="787">
       <c r="A787" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="788">
@@ -4392,7 +4392,7 @@
     </row>
     <row r="792">
       <c r="A792" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="793">
@@ -4427,7 +4427,7 @@
     </row>
     <row r="799">
       <c r="A799" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="800">
@@ -4447,7 +4447,7 @@
     </row>
     <row r="803">
       <c r="A803" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="804">
@@ -4467,17 +4467,17 @@
     </row>
     <row r="807">
       <c r="A807" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="808">
       <c r="A808" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="809">
       <c r="A809" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="810">
@@ -4537,7 +4537,7 @@
     </row>
     <row r="821">
       <c r="A821" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="822">
@@ -4607,7 +4607,7 @@
     </row>
     <row r="835">
       <c r="A835" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="836">

</xml_diff>

<commit_message>
Update output Excel files with new data and analysis results
- Updated control energy QC summary
- Updated control set maps for bipolar and monopolar configurations (k1, k3)
- Updated top 1 outliers for control and monopolar datasets
- Updated NCT outputs bundle
- Updated node energy by group
- Updated sEEG bipolar and monopolar data aligned to B0 and MNI
</commit_message>
<xml_diff>
--- a/output/B_vector_diag.xlsx
+++ b/output/B_vector_diag.xlsx
@@ -472,7 +472,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -602,7 +602,7 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -682,7 +682,7 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -707,7 +707,7 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -737,7 +737,7 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -747,7 +747,7 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -762,7 +762,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -772,7 +772,7 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -967,7 +967,7 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
@@ -1022,7 +1022,7 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -1087,12 +1087,12 @@
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
@@ -1167,7 +1167,7 @@
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -1212,7 +1212,7 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -1227,7 +1227,7 @@
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
@@ -1267,7 +1267,7 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -1297,7 +1297,7 @@
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174">
@@ -1307,12 +1307,12 @@
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -1427,7 +1427,7 @@
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200">
@@ -1532,7 +1532,7 @@
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221">
@@ -1542,7 +1542,7 @@
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="223">
@@ -1737,7 +1737,7 @@
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="262">
@@ -1907,12 +1907,12 @@
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="297">
@@ -1932,7 +1932,7 @@
     </row>
     <row r="300">
       <c r="A300" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="301">
@@ -2037,7 +2037,7 @@
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="322">
@@ -2072,7 +2072,7 @@
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="329">
@@ -2177,7 +2177,7 @@
     </row>
     <row r="349">
       <c r="A349" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="350">
@@ -2382,7 +2382,7 @@
     </row>
     <row r="390">
       <c r="A390" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="391">
@@ -2397,7 +2397,7 @@
     </row>
     <row r="393">
       <c r="A393" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="394">
@@ -2432,7 +2432,7 @@
     </row>
     <row r="400">
       <c r="A400" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="401">
@@ -2477,7 +2477,7 @@
     </row>
     <row r="409">
       <c r="A409" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="410">
@@ -2522,7 +2522,7 @@
     </row>
     <row r="418">
       <c r="A418" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="419">
@@ -2922,7 +2922,7 @@
     </row>
     <row r="498">
       <c r="A498" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="499">
@@ -3167,7 +3167,7 @@
     </row>
     <row r="547">
       <c r="A547" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="548">
@@ -4052,7 +4052,7 @@
     </row>
     <row r="724">
       <c r="A724" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="725">
@@ -4237,7 +4237,7 @@
     </row>
     <row r="761">
       <c r="A761" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="762">
@@ -4247,7 +4247,7 @@
     </row>
     <row r="763">
       <c r="A763" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="764">
@@ -4417,7 +4417,7 @@
     </row>
     <row r="797">
       <c r="A797" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="798">
@@ -4427,7 +4427,7 @@
     </row>
     <row r="799">
       <c r="A799" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="800">

</xml_diff>